<commit_message>
Third storage power cost as transmission
</commit_message>
<xml_diff>
--- a/all_firm_case.xlsx
+++ b/all_firm_case.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/Library/Group Containers/G69SCX94XU.duck/Library/Application Support/duck/Volumes.noindex/DPB-DGE Data Transfer Node/nobackup/scratch/awongel/clab_all_firm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_all_firm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECB34B9-06D4-4F48-89A7-892D3DEE3C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB61AB0-215F-EC4F-8C60-F457E29E2856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="500" windowWidth="27920" windowHeight="15020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_intermodel_one_node_" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="137">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -410,9 +410,6 @@
     <t>biopower</t>
   </si>
   <si>
-    <t>phs_energy</t>
-  </si>
-  <si>
     <t>phs_power</t>
   </si>
   <si>
@@ -428,19 +425,31 @@
     <t>US_demand_unnormalized.csv</t>
   </si>
   <si>
-    <t>/carnegie/data/Shared/Labs/Caldeira Lab/Everyone/energy_demand_capacity_data/US_solar_wind_demand/</t>
-  </si>
-  <si>
     <t>all_firm_case</t>
   </si>
   <si>
-    <t>all_firm</t>
-  </si>
-  <si>
     <t>#Generator</t>
   </si>
   <si>
     <t>Decay rate</t>
+  </si>
+  <si>
+    <t>/Volumes/Shared/Labs/Caldeira Lab/Everyone/energy_demand_capacity_data/US_solar_wind_demand/</t>
+  </si>
+  <si>
+    <t>all_firm_all</t>
+  </si>
+  <si>
+    <t>third_storage</t>
+  </si>
+  <si>
+    <t>p_min_pu</t>
+  </si>
+  <si>
+    <t>Note: p_min_mu sets uni/bidirectionality</t>
+  </si>
+  <si>
+    <t>phs</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1023,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1067,7 +1076,6 @@
     <xf numFmtId="49" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1078,7 +1086,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="43"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1489,10 +1496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S103"/>
+  <dimension ref="A1:T103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O61" sqref="O61"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1768,7 +1775,7 @@
         <v>45</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1784,7 +1791,7 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1792,7 +1799,7 @@
         <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1837,7 +1844,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>96</v>
       </c>
@@ -1846,11 +1853,11 @@
         <v>8784</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -1862,7 +1869,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1874,11 +1881,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -1887,7 +1894,7 @@
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -1896,7 +1903,7 @@
       </c>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -1905,19 +1912,22 @@
       </c>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>18</v>
       </c>
+      <c r="F42" t="s">
+        <v>135</v>
+      </c>
       <c r="J42" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D43" t="s">
         <v>73</v>
       </c>
@@ -1928,12 +1938,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:19" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>4</v>
       </c>
@@ -1943,35 +1953,35 @@
       <c r="D45" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H45" s="4" t="s">
+      <c r="I45" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I45" s="4" t="s">
+      <c r="J45" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J45" s="4" t="s">
+      <c r="K45" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L45" s="4" t="s">
+      <c r="M45" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N45" s="4" t="s">
+      <c r="O45" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P45" s="5" t="s">
+      <c r="Q45" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q45" s="5" t="s">
+      <c r="R45" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R45" s="5"/>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S45" s="5"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:19" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>20</v>
       </c>
@@ -1988,37 +1998,40 @@
         <v>37</v>
       </c>
       <c r="F47" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="H47" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="I47" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="J47" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="L47" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M47" s="2" t="s">
+      <c r="N47" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N47" s="2" t="s">
+      <c r="O47" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O47" s="2" t="s">
+      <c r="P47" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P47" s="2" t="s">
+      <c r="Q47" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="Q47" s="2" t="s">
+      <c r="R47" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>53</v>
       </c>
@@ -2031,20 +2044,20 @@
       <c r="D48" t="s">
         <v>22</v>
       </c>
-      <c r="F48" t="s">
-        <v>128</v>
-      </c>
-      <c r="I48" s="26"/>
-      <c r="K48" s="15"/>
-      <c r="R48" t="str">
+      <c r="G48" t="s">
+        <v>127</v>
+      </c>
+      <c r="J48" s="26"/>
+      <c r="L48" s="15"/>
+      <c r="S48" t="str">
         <f xml:space="preserve"> 1 &amp; "/" &amp; B38</f>
         <v>1/h</v>
       </c>
-      <c r="S48" t="s">
+      <c r="T48" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>52</v>
       </c>
@@ -2057,24 +2070,24 @@
       <c r="D49" t="s">
         <v>22</v>
       </c>
-      <c r="F49" t="s">
-        <v>126</v>
-      </c>
-      <c r="I49" s="26">
+      <c r="G49" t="s">
+        <v>125</v>
+      </c>
+      <c r="J49" s="26">
         <f>N85*B33</f>
         <v>135.46581245459663</v>
       </c>
-      <c r="J49" t="str">
+      <c r="K49" t="str">
         <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K49" s="15"/>
-      <c r="L49" t="str">
+      <c r="L49" s="15"/>
+      <c r="M49" t="str">
         <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>52</v>
       </c>
@@ -2087,26 +2100,26 @@
       <c r="D50" t="s">
         <v>22</v>
       </c>
-      <c r="F50" t="s">
-        <v>127</v>
-      </c>
-      <c r="I50" s="26">
+      <c r="G50" t="s">
+        <v>126</v>
+      </c>
+      <c r="J50" s="26">
         <f>N86*B33</f>
         <v>159.15693044316652</v>
       </c>
-      <c r="J50" t="str">
+      <c r="K50" t="str">
         <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K50" s="15"/>
-      <c r="L50" t="str">
+      <c r="L50" s="15"/>
+      <c r="M50" t="str">
         <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B51" t="s">
         <v>29</v>
@@ -2117,24 +2130,24 @@
       <c r="D51" t="s">
         <v>22</v>
       </c>
-      <c r="I51" s="26">
+      <c r="J51" s="26">
         <f>N87*B33</f>
         <v>112.24474894263096</v>
       </c>
-      <c r="J51" t="str">
+      <c r="K51" t="str">
         <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K51" s="15">
+      <c r="L51" s="15">
         <f>I87 + J87/L87</f>
         <v>1.6911456050362664E-2</v>
       </c>
-      <c r="L51" t="str">
+      <c r="M51" t="str">
         <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>52</v>
       </c>
@@ -2147,24 +2160,24 @@
       <c r="D52" t="s">
         <v>22</v>
       </c>
-      <c r="I52" s="27">
+      <c r="J52" s="27">
         <f>N88*B33</f>
         <v>280.93327462774823</v>
       </c>
-      <c r="J52" t="str">
+      <c r="K52" t="str">
         <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K52" s="15">
+      <c r="L52" s="15">
         <f>I88 + J88/L88</f>
         <v>1.8144865147936888E-2</v>
       </c>
-      <c r="L52" t="str">
+      <c r="M52" t="str">
         <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>52</v>
       </c>
@@ -2177,24 +2190,24 @@
       <c r="D53" t="s">
         <v>22</v>
       </c>
-      <c r="I53" s="26">
+      <c r="J53" s="26">
         <f>N89*B33</f>
         <v>742.40076653499398</v>
       </c>
-      <c r="J53" t="str">
+      <c r="K53" t="str">
         <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K53" s="15">
+      <c r="L53" s="15">
         <f>I89 + J89/L89</f>
         <v>2.3458663758010111E-2</v>
       </c>
-      <c r="L53" t="str">
+      <c r="M53" t="str">
         <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
         <v>52</v>
       </c>
@@ -2207,23 +2220,23 @@
       <c r="D54" t="s">
         <v>22</v>
       </c>
-      <c r="I54" s="26">
+      <c r="J54" s="26">
         <f>N90*B33</f>
         <v>501.59899872684895</v>
       </c>
-      <c r="J54" t="str">
+      <c r="K54" t="str">
         <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K54" s="15"/>
-      <c r="L54" t="str">
+      <c r="L54" s="15"/>
+      <c r="M54" t="str">
         <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B55" t="s">
         <v>103</v>
@@ -2234,10 +2247,10 @@
       <c r="D55" t="s">
         <v>22</v>
       </c>
-      <c r="I55" s="26"/>
-      <c r="K55" s="15"/>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J55" s="26"/>
+      <c r="L55" s="15"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>52</v>
       </c>
@@ -2250,21 +2263,21 @@
       <c r="D56" t="s">
         <v>22</v>
       </c>
-      <c r="I56" s="27">
+      <c r="J56" s="27">
         <f>N92*B33</f>
         <v>1883.019444812541</v>
       </c>
-      <c r="J56" t="str">
+      <c r="K56" t="str">
         <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K56" s="15"/>
-      <c r="L56" t="str">
+      <c r="L56" s="15"/>
+      <c r="M56" t="str">
         <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
         <v>54</v>
       </c>
@@ -2277,34 +2290,34 @@
       <c r="D57" t="s">
         <v>22</v>
       </c>
-      <c r="I57" s="27">
+      <c r="J57" s="27">
         <f>(N93+N94)*B33</f>
         <v>56.563262262275956</v>
       </c>
-      <c r="J57" t="str">
+      <c r="K57" t="str">
         <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K57" s="15">
+      <c r="L57" s="15">
         <f>P94</f>
         <v>3.1E-6</v>
       </c>
-      <c r="L57" t="str">
+      <c r="M57" t="str">
         <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
       </c>
-      <c r="M57">
+      <c r="N57">
         <v>4</v>
       </c>
-      <c r="N57" t="b">
+      <c r="O57" t="b">
         <v>1</v>
       </c>
-      <c r="O57">
+      <c r="P57">
         <f>L94</f>
         <v>0.86</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
         <v>91</v>
       </c>
@@ -2320,28 +2333,31 @@
       <c r="E58" t="s">
         <v>38</v>
       </c>
-      <c r="I58" s="26">
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="J58" s="26">
         <f>N95*B33</f>
         <v>153.0544177167759</v>
       </c>
-      <c r="J58" t="str">
+      <c r="K58" t="str">
         <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K58" s="15">
+      <c r="L58" s="15">
         <f>P95</f>
         <v>1.2999999999999998E-6</v>
       </c>
-      <c r="L58" t="str">
+      <c r="M58" t="str">
         <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
       </c>
-      <c r="O58">
+      <c r="P58">
         <f>L95</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>92</v>
       </c>
@@ -2354,25 +2370,25 @@
       <c r="D59" t="s">
         <v>38</v>
       </c>
-      <c r="I59" s="26">
+      <c r="J59" s="26">
         <f>N96*B33</f>
         <v>0.16397297656507703</v>
       </c>
-      <c r="J59" t="str">
+      <c r="K59" t="str">
         <f>B40 &amp; "/time range/" &amp; B39 &amp; B38</f>
         <v>$/time range/kWh</v>
       </c>
-      <c r="K59" s="15"/>
-      <c r="L59" t="str">
+      <c r="L59" s="15"/>
+      <c r="M59" t="str">
         <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
       </c>
-      <c r="Q59">
+      <c r="R59">
         <f>M96</f>
         <v>4.1666666666666665E-5</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>91</v>
       </c>
@@ -2388,83 +2404,96 @@
       <c r="E60" t="s">
         <v>22</v>
       </c>
-      <c r="I60" s="26">
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="J60" s="26">
         <f>N97*B33</f>
         <v>129.12774868738202</v>
       </c>
-      <c r="J60" t="str">
+      <c r="K60" t="str">
         <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K60" s="15">
+      <c r="L60" s="15">
         <f>P97</f>
         <v>5.1249999999999993E-4</v>
       </c>
-      <c r="L60" t="str">
+      <c r="M60" t="str">
         <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
       </c>
-      <c r="O60">
+      <c r="P60">
         <f>L97</f>
         <v>0.71</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="C61" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="D61" t="s">
         <v>22</v>
       </c>
-      <c r="I61" s="27">
+      <c r="J61" s="27">
         <f>N98*B33</f>
         <v>8.6253132060507376</v>
       </c>
-      <c r="J61" t="str">
+      <c r="K61" t="str">
         <f>B40 &amp; "/time range/" &amp; B39 &amp; B38</f>
         <v>$/time range/kWh</v>
       </c>
-      <c r="K61" s="15"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L61" s="15"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
       </c>
-      <c r="I62" s="27">
+      <c r="E62" t="s">
+        <v>133</v>
+      </c>
+      <c r="F62">
+        <v>-1</v>
+      </c>
+      <c r="J62" s="27">
         <f>N99*B33</f>
         <v>147.6443387634331</v>
       </c>
-      <c r="J62" t="str">
+      <c r="K62" t="str">
         <f>B40 &amp; "/time range/" &amp; B39</f>
         <v>$/time range/kW</v>
       </c>
-      <c r="K62" s="15">
+      <c r="L62" s="15">
         <f>P99</f>
         <v>2.9999999999999999E-7</v>
       </c>
-      <c r="L62" t="str">
+      <c r="M62" t="str">
         <f xml:space="preserve"> B40 &amp; "/" &amp; B39 &amp; B38</f>
         <v>$/kWh</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P62">
+        <f>L99</f>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B63" t="s">
         <v>100</v>
@@ -2478,8 +2507,8 @@
       <c r="E63" t="s">
         <v>101</v>
       </c>
-      <c r="I63" s="26"/>
-      <c r="K63" s="15"/>
+      <c r="J63" s="26"/>
+      <c r="L63" s="15"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
@@ -2529,10 +2558,10 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="12"/>
-      <c r="B74" s="30" t="s">
+      <c r="B74" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="C74" s="29" t="s">
+      <c r="C74" s="28" t="s">
         <v>107</v>
       </c>
       <c r="E74" s="11"/>
@@ -2548,10 +2577,10 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="12"/>
-      <c r="B75" s="30" t="s">
+      <c r="B75" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="C75" s="29" t="s">
+      <c r="C75" s="28" t="s">
         <v>110</v>
       </c>
       <c r="E75" s="11"/>
@@ -2567,8 +2596,8 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="12"/>
-      <c r="B76" s="30"/>
-      <c r="C76" s="29"/>
+      <c r="B76" s="29"/>
+      <c r="C76" s="28"/>
       <c r="E76" s="11"/>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
@@ -2582,10 +2611,10 @@
     </row>
     <row r="77" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="12"/>
-      <c r="B77" s="30" t="s">
+      <c r="B77" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="C77" s="31" t="s">
+      <c r="C77" s="30" t="s">
         <v>112</v>
       </c>
       <c r="E77" s="11"/>
@@ -2601,8 +2630,8 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="12"/>
-      <c r="B78" s="29"/>
-      <c r="C78" s="32" t="s">
+      <c r="B78" s="28"/>
+      <c r="C78" s="31" t="s">
         <v>113</v>
       </c>
       <c r="E78" s="11"/>
@@ -2618,8 +2647,8 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="12"/>
-      <c r="B79" s="29"/>
-      <c r="C79" s="32"/>
+      <c r="B79" s="28"/>
+      <c r="C79" s="31"/>
       <c r="E79" s="11"/>
       <c r="F79" s="11"/>
       <c r="G79" s="11"/>
@@ -2631,34 +2660,34 @@
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
     </row>
-    <row r="80" spans="1:14" s="40" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="37"/>
-      <c r="B80" s="38" t="s">
+    <row r="80" spans="1:14" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="35"/>
+      <c r="B80" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="C80" s="39"/>
-      <c r="E80" s="41"/>
-      <c r="F80" s="41"/>
-      <c r="G80" s="41"/>
-      <c r="H80" s="41"/>
-      <c r="I80" s="41"/>
-      <c r="J80" s="41"/>
-      <c r="K80" s="41"/>
-      <c r="L80" s="41"/>
-      <c r="M80" s="42"/>
-      <c r="N80" s="42"/>
+      <c r="C80" s="37"/>
+      <c r="E80" s="39"/>
+      <c r="F80" s="39"/>
+      <c r="G80" s="39"/>
+      <c r="H80" s="39"/>
+      <c r="I80" s="39"/>
+      <c r="J80" s="39"/>
+      <c r="K80" s="39"/>
+      <c r="L80" s="39"/>
+      <c r="M80" s="40"/>
+      <c r="N80" s="40"/>
     </row>
     <row r="81" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="12"/>
-      <c r="B81" s="35" t="s">
+      <c r="B81" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="C81" s="36">
+      <c r="C81" s="34">
         <v>1.02</v>
       </c>
-      <c r="D81" s="34"/>
-      <c r="E81" s="34"/>
-      <c r="F81" s="34"/>
+      <c r="D81" s="32"/>
+      <c r="E81" s="32"/>
+      <c r="F81" s="32"/>
       <c r="G81" s="14"/>
       <c r="H81" s="16"/>
       <c r="I81" s="16"/>
@@ -2760,7 +2789,7 @@
         <v>85</v>
       </c>
       <c r="M84" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="N84" s="19" t="s">
         <v>51</v>
@@ -2790,7 +2819,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="H85" s="18">
-        <f>C85*G85+D85</f>
+        <f t="shared" ref="H85:H90" si="0">C85*G85+D85</f>
         <v>135.09568728395567</v>
       </c>
       <c r="I85" s="14"/>
@@ -2799,7 +2828,7 @@
       <c r="L85" s="14"/>
       <c r="M85" s="14"/>
       <c r="N85" s="20">
-        <f>H85/8760</f>
+        <f t="shared" ref="N85:N90" si="1">H85/8760</f>
         <v>1.5421882110040601E-2</v>
       </c>
       <c r="O85" s="14" t="str">
@@ -2831,7 +2860,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="H86" s="18">
-        <f>C86*G86+D86</f>
+        <f t="shared" si="0"/>
         <v>158.72207544195567</v>
       </c>
       <c r="I86" s="14"/>
@@ -2840,7 +2869,7 @@
       <c r="L86" s="14"/>
       <c r="M86" s="14"/>
       <c r="N86" s="20">
-        <f>H86/8760</f>
+        <f t="shared" si="1"/>
         <v>1.8118958383784894E-2</v>
       </c>
       <c r="O86" s="14" t="str">
@@ -2872,7 +2901,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="H87" s="18">
-        <f>C87*G87+D87</f>
+        <f t="shared" si="0"/>
         <v>111.93806930071121</v>
       </c>
       <c r="I87" s="14">
@@ -2890,7 +2919,7 @@
       </c>
       <c r="M87" s="14"/>
       <c r="N87" s="20">
-        <f>H87/8760</f>
+        <f t="shared" si="1"/>
         <v>1.2778318413323197E-2</v>
       </c>
       <c r="O87" s="14" t="str">
@@ -2910,14 +2939,14 @@
       <c r="B88" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C88" s="33">
+      <c r="C88" s="20">
         <v>2670</v>
       </c>
-      <c r="D88" s="28">
+      <c r="D88" s="14">
         <v>65</v>
       </c>
-      <c r="E88" s="28"/>
-      <c r="F88" s="28">
+      <c r="E88" s="14"/>
+      <c r="F88" s="14">
         <v>30</v>
       </c>
       <c r="G88" s="14">
@@ -2925,7 +2954,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="H88" s="18">
-        <f>C88*G88+D88</f>
+        <f t="shared" si="0"/>
         <v>280.16569737466693</v>
       </c>
       <c r="I88" s="14">
@@ -2943,7 +2972,7 @@
       </c>
       <c r="M88" s="14"/>
       <c r="N88" s="20">
-        <f>H88/8760</f>
+        <f t="shared" si="1"/>
         <v>3.1982385545053303E-2</v>
       </c>
       <c r="O88" s="14" t="str">
@@ -2978,7 +3007,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="H89" s="18">
-        <f>C89*G89+D89</f>
+        <f t="shared" si="0"/>
         <v>740.37234914008957</v>
       </c>
       <c r="I89" s="14">
@@ -2996,7 +3025,7 @@
       </c>
       <c r="M89" s="14"/>
       <c r="N89" s="20">
-        <f>H89/8760</f>
+        <f t="shared" si="1"/>
         <v>8.4517391454348126E-2</v>
       </c>
       <c r="O89" s="14" t="str">
@@ -3031,7 +3060,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="H90" s="18">
-        <f>C90*G90+D90</f>
+        <f t="shared" si="0"/>
         <v>500.22850965928927</v>
       </c>
       <c r="I90" s="14">
@@ -3049,7 +3078,7 @@
       </c>
       <c r="M90" s="14"/>
       <c r="N90" s="20">
-        <f>H90/8760</f>
+        <f t="shared" si="1"/>
         <v>5.7103711148320691E-2</v>
       </c>
       <c r="O90" s="14" t="str">
@@ -3187,7 +3216,7 @@
         <f>8.3*C81</f>
         <v>8.4660000000000011</v>
       </c>
-      <c r="E94" s="43">
+      <c r="E94" s="41">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F94" s="14">
@@ -3236,7 +3265,7 @@
         <f>12.8*C81</f>
         <v>13.056000000000001</v>
       </c>
-      <c r="E95" s="43">
+      <c r="E95" s="41">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F95" s="14">
@@ -3247,7 +3276,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="H95" s="18">
-        <f t="shared" ref="H95:H99" si="0">(C95+E95*C95)*G95+D95</f>
+        <f t="shared" ref="H95:H99" si="2">(C95+E95*C95)*G95+D95</f>
         <v>152.63623624760439</v>
       </c>
       <c r="I95" s="14"/>
@@ -3258,7 +3287,7 @@
       </c>
       <c r="M95" s="14"/>
       <c r="N95" s="20">
-        <f t="shared" ref="N95:N99" si="1">H95/8760</f>
+        <f t="shared" ref="N95:N99" si="3">H95/8760</f>
         <v>1.742422788214662E-2</v>
       </c>
       <c r="O95" s="14" t="str">
@@ -3306,7 +3335,7 @@
         <v>4.1666666666666665E-5</v>
       </c>
       <c r="N96" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.8667233215514235E-5</v>
       </c>
       <c r="O96" s="14" t="str">
@@ -3331,7 +3360,7 @@
         <f>12.8*C81</f>
         <v>13.056000000000001</v>
       </c>
-      <c r="E97" s="43">
+      <c r="E97" s="41">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F97" s="14">
@@ -3342,7 +3371,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="H97" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>128.77494063085911</v>
       </c>
       <c r="I97" s="14"/>
@@ -3353,7 +3382,7 @@
       </c>
       <c r="M97" s="14"/>
       <c r="N97" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.4700335688454236E-2</v>
       </c>
       <c r="O97" s="14" t="str">
@@ -3398,7 +3427,7 @@
       <c r="L98" s="14"/>
       <c r="M98" s="14"/>
       <c r="N98" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.8193456353036631E-4</v>
       </c>
       <c r="O98" s="14"/>
@@ -3420,7 +3449,7 @@
         <f>12.5*C81</f>
         <v>12.75</v>
       </c>
-      <c r="E99" s="43">
+      <c r="E99" s="41">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F99" s="14">
@@ -3431,7 +3460,7 @@
         <v>8.0586403511111196E-2</v>
       </c>
       <c r="H99" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>147.24093893074613</v>
       </c>
       <c r="I99" s="20"/>
@@ -3442,7 +3471,7 @@
       </c>
       <c r="M99" s="14"/>
       <c r="N99" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.680832636195732E-2</v>
       </c>
       <c r="O99" s="14"/>

</xml_diff>

<commit_message>
update for leaast cost increase
</commit_message>
<xml_diff>
--- a/all_firm_case.xlsx
+++ b/all_firm_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/CLab/clab_all_firm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/Library/Group Containers/G69SCX94XU.duck/Library/Application Support/duck/Volumes.noindex/DPB-DGE Data Transfer Node/nobackup/scratch/awongel/clab_all_firm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA64321-580B-6F42-B022-E7DD136808A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD4D686-A7DD-774C-9F77-24E46BF2C77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="4140" windowWidth="34940" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_intermodel_one_node_" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="197">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -288,9 +288,6 @@
     <t>US_demand_unnormalized.csv</t>
   </si>
   <si>
-    <t>/Volumes/Shared/Labs/Caldeira Lab/Everyone/energy_demand_capacity_data/US_solar_wind_demand/</t>
-  </si>
-  <si>
     <t>p_min_pu</t>
   </si>
   <si>
@@ -342,283 +339,295 @@
     <t>https://raw.githubusercontent.com/PyPSA/technology-data/master/outputs/costs_2020.csv</t>
   </si>
   <si>
+    <t>direct air capture</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>onwind</t>
+  </si>
+  <si>
+    <t>Note: To use PyPSA default costs, use same technology names as in costs_path</t>
+  </si>
+  <si>
+    <t>hydro</t>
+  </si>
+  <si>
+    <t>fuel cell</t>
+  </si>
+  <si>
+    <t>battery storage</t>
+  </si>
+  <si>
+    <t>co2_emissions</t>
+  </si>
+  <si>
+    <t>2017-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>CO2 storage tank</t>
+  </si>
+  <si>
+    <t>hydrogen storage underground</t>
+  </si>
+  <si>
+    <t>solar-utility</t>
+  </si>
+  <si>
+    <t>Note: costing for nuclear heat has to be for kWh thermal (or other energy unit)</t>
+  </si>
+  <si>
+    <t>Note: % indicates addition to standard PyPSA name which stands before the %</t>
+  </si>
+  <si>
+    <t>CCGT % link</t>
+  </si>
+  <si>
+    <t>phs power</t>
+  </si>
+  <si>
+    <t>phs energy</t>
+  </si>
+  <si>
+    <t>Cost calculations</t>
+  </si>
+  <si>
+    <t>Hunter et al. Techno-Economic Analysis of Long-Duration Energy Storage and Flexible Power Generation Technologies to Support High-Variable Renewable Energy Grids. Joule 2021, 5 (8), 2077–2101.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://doi.org/10.1016/j.joule.2021.06.018.</t>
+  </si>
+  <si>
+    <t>Discount rate</t>
+  </si>
+  <si>
+    <t>Other fixed cost* (% of capital cost)</t>
+  </si>
+  <si>
+    <t>Lifetime [years]</t>
+  </si>
+  <si>
+    <t>Capital recovery factor [%/year]</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Decay rate</t>
+  </si>
+  <si>
+    <t>Hourly fixed costs</t>
+  </si>
+  <si>
+    <t>pumped_hydro_storage energy</t>
+  </si>
+  <si>
+    <t>pumped_hydro_storage power</t>
+  </si>
+  <si>
+    <t>* includes property, tax, insurance, licensing, permiting costs</t>
+  </si>
+  <si>
+    <t>carrier</t>
+  </si>
+  <si>
+    <t>Note: carrier allows to group different technologies</t>
+  </si>
+  <si>
+    <t>hydrogen</t>
+  </si>
+  <si>
+    <t>phs</t>
+  </si>
+  <si>
+    <t>natgas</t>
+  </si>
+  <si>
+    <t>load shifting forward</t>
+  </si>
+  <si>
+    <t>load shifting backward</t>
+  </si>
+  <si>
+    <t>Note: cost per energy stored for Store/StoragUnit</t>
+  </si>
+  <si>
+    <t>p_max_pu</t>
+  </si>
+  <si>
+    <t>sign</t>
+  </si>
+  <si>
+    <t>Source load shifting costs</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.20357/B7MS40</t>
+  </si>
+  <si>
+    <t>Gerke et al. The California Demand Response Potential Study, Phase 3: Final Report on the Shift Resource through 2030.</t>
+  </si>
+  <si>
+    <t>https://github.com/PyPSA/technology-data/blob/master/outputs/costs_2020.csv</t>
+  </si>
+  <si>
+    <t>PyPSA technology data</t>
+  </si>
+  <si>
+    <t>Source PHS costs</t>
+  </si>
+  <si>
+    <t>Source all other costs</t>
+  </si>
+  <si>
+    <t>Source natural gas CCS costs</t>
+  </si>
+  <si>
+    <t>natural gas with CCS</t>
+  </si>
+  <si>
+    <t>(NG combined cycle 95% CCS (H-frame basis -&gt; 2nd Gen Tech)), Moderate</t>
+  </si>
+  <si>
+    <t>co2 atmosphere</t>
+  </si>
+  <si>
+    <t>load shedding</t>
+  </si>
+  <si>
+    <t>solver</t>
+  </si>
+  <si>
+    <t>gurobi</t>
+  </si>
+  <si>
+    <t>CCGT % wCCS</t>
+  </si>
+  <si>
+    <t>CCGT % link wCCS</t>
+  </si>
+  <si>
+    <t>.05*co2_emissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCGT </t>
+  </si>
+  <si>
+    <t>load shifting</t>
+  </si>
+  <si>
+    <t>geothermal % link</t>
+  </si>
+  <si>
+    <t>geoth_out</t>
+  </si>
+  <si>
+    <t>-1*energy-input</t>
+  </si>
+  <si>
+    <t>natgas_wCCS</t>
+  </si>
+  <si>
+    <t>Note: Path to PyPSA database</t>
+  </si>
+  <si>
+    <t>Data source</t>
+  </si>
+  <si>
+    <t>PyPSA DB</t>
+  </si>
+  <si>
+    <t>Hunter et al</t>
+  </si>
+  <si>
+    <t>Gerke et al</t>
+  </si>
+  <si>
+    <t>NREL</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>€</t>
+  </si>
+  <si>
+    <t>Note: 2020 €</t>
+  </si>
+  <si>
+    <t>2020 €/$</t>
+  </si>
+  <si>
+    <t>BECCS</t>
+  </si>
+  <si>
+    <t>Source lost load</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.tej.2022.107187</t>
+  </si>
+  <si>
+    <t>Gorman. The quest to quantify the value of lost load: A critical review of the economics of power outages</t>
+  </si>
+  <si>
+    <t>https://atb-archive.nrel.gov/electricity/2020/data.php</t>
+  </si>
+  <si>
+    <t>NREL (National Renewable Energy Laboratory). 2020. "2020 Annual Technology Baseline."</t>
+  </si>
+  <si>
+    <t>Source BECCS</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/docs/fy22osti/81644.pdf</t>
+  </si>
+  <si>
+    <t>CO2 emissions</t>
+  </si>
+  <si>
+    <t>tCO2/MWh</t>
+  </si>
+  <si>
+    <t>BECCS % link</t>
+  </si>
+  <si>
+    <t>beccs</t>
+  </si>
+  <si>
+    <t>beccs_out</t>
+  </si>
+  <si>
+    <t>Gorman</t>
+  </si>
+  <si>
+    <t>natgas_wCCS_out</t>
+  </si>
+  <si>
+    <t>Variable cost [€/MWh]</t>
+  </si>
+  <si>
+    <t>/carnegie/data/Shared/Labs/Caldeira Lab/Everyone/energy_demand_capacity_data/US_solar_wind_demand/</t>
+  </si>
+  <si>
+    <t>StorageUnit</t>
+  </si>
+  <si>
+    <t>all_firm</t>
+  </si>
+  <si>
+    <t>(1.14)</t>
+  </si>
+  <si>
+    <t>#Generator</t>
+  </si>
+  <si>
+    <t>#Link</t>
+  </si>
+  <si>
+    <t>all_firm_case_cost_removal_no_geo_hydro</t>
+  </si>
+  <si>
     <t>info</t>
-  </si>
-  <si>
-    <t>direct air capture</t>
-  </si>
-  <si>
-    <t>MW</t>
-  </si>
-  <si>
-    <t>onwind</t>
-  </si>
-  <si>
-    <t>Note: To use PyPSA default costs, use same technology names as in costs_path</t>
-  </si>
-  <si>
-    <t>hydro</t>
-  </si>
-  <si>
-    <t>fuel cell</t>
-  </si>
-  <si>
-    <t>battery storage</t>
-  </si>
-  <si>
-    <t>StorageUnit</t>
-  </si>
-  <si>
-    <t>co2_emissions</t>
-  </si>
-  <si>
-    <t>2017-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>CO2 storage tank</t>
-  </si>
-  <si>
-    <t>hydrogen storage underground</t>
-  </si>
-  <si>
-    <t>solar-utility</t>
-  </si>
-  <si>
-    <t>Note: costing for nuclear heat has to be for kWh thermal (or other energy unit)</t>
-  </si>
-  <si>
-    <t>Note: % indicates addition to standard PyPSA name which stands before the %</t>
-  </si>
-  <si>
-    <t>CCGT % link</t>
-  </si>
-  <si>
-    <t>phs power</t>
-  </si>
-  <si>
-    <t>phs energy</t>
-  </si>
-  <si>
-    <t>Cost calculations</t>
-  </si>
-  <si>
-    <t>Hunter et al. Techno-Economic Analysis of Long-Duration Energy Storage and Flexible Power Generation Technologies to Support High-Variable Renewable Energy Grids. Joule 2021, 5 (8), 2077–2101.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> https://doi.org/10.1016/j.joule.2021.06.018.</t>
-  </si>
-  <si>
-    <t>Discount rate</t>
-  </si>
-  <si>
-    <t>Other fixed cost* (% of capital cost)</t>
-  </si>
-  <si>
-    <t>Lifetime [years]</t>
-  </si>
-  <si>
-    <t>Capital recovery factor [%/year]</t>
-  </si>
-  <si>
-    <t>Efficiency</t>
-  </si>
-  <si>
-    <t>Decay rate</t>
-  </si>
-  <si>
-    <t>Hourly fixed costs</t>
-  </si>
-  <si>
-    <t>pumped_hydro_storage energy</t>
-  </si>
-  <si>
-    <t>pumped_hydro_storage power</t>
-  </si>
-  <si>
-    <t>* includes property, tax, insurance, licensing, permiting costs</t>
-  </si>
-  <si>
-    <t>carrier</t>
-  </si>
-  <si>
-    <t>Note: carrier allows to group different technologies</t>
-  </si>
-  <si>
-    <t>hydrogen</t>
-  </si>
-  <si>
-    <t>phs</t>
-  </si>
-  <si>
-    <t>natgas</t>
-  </si>
-  <si>
-    <t>load shifting forward</t>
-  </si>
-  <si>
-    <t>load shifting backward</t>
-  </si>
-  <si>
-    <t>Note: cost per energy stored for Store/StoragUnit</t>
-  </si>
-  <si>
-    <t>p_max_pu</t>
-  </si>
-  <si>
-    <t>sign</t>
-  </si>
-  <si>
-    <t>all_firm</t>
-  </si>
-  <si>
-    <t>Source load shifting costs</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.20357/B7MS40</t>
-  </si>
-  <si>
-    <t>Gerke et al. The California Demand Response Potential Study, Phase 3: Final Report on the Shift Resource through 2030.</t>
-  </si>
-  <si>
-    <t>https://github.com/PyPSA/technology-data/blob/master/outputs/costs_2020.csv</t>
-  </si>
-  <si>
-    <t>PyPSA technology data</t>
-  </si>
-  <si>
-    <t>Source PHS costs</t>
-  </si>
-  <si>
-    <t>Source all other costs</t>
-  </si>
-  <si>
-    <t>Source natural gas CCS costs</t>
-  </si>
-  <si>
-    <t>natural gas with CCS</t>
-  </si>
-  <si>
-    <t>(NG combined cycle 95% CCS (H-frame basis -&gt; 2nd Gen Tech)), Moderate</t>
-  </si>
-  <si>
-    <t>co2 atmosphere</t>
-  </si>
-  <si>
-    <t>load shedding</t>
-  </si>
-  <si>
-    <t>solver</t>
-  </si>
-  <si>
-    <t>gurobi</t>
-  </si>
-  <si>
-    <t>CCGT % wCCS</t>
-  </si>
-  <si>
-    <t>CCGT % link wCCS</t>
-  </si>
-  <si>
-    <t>.05*co2_emissions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCGT </t>
-  </si>
-  <si>
-    <t>load shifting</t>
-  </si>
-  <si>
-    <t>geothermal % link</t>
-  </si>
-  <si>
-    <t>geoth_out</t>
-  </si>
-  <si>
-    <t>-1*energy-input</t>
-  </si>
-  <si>
-    <t>natgas_wCCS</t>
-  </si>
-  <si>
-    <t>Note: Path to PyPSA database</t>
-  </si>
-  <si>
-    <t>Data source</t>
-  </si>
-  <si>
-    <t>PyPSA DB</t>
-  </si>
-  <si>
-    <t>Hunter et al</t>
-  </si>
-  <si>
-    <t>Gerke et al</t>
-  </si>
-  <si>
-    <t>NREL</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>€</t>
-  </si>
-  <si>
-    <t>Note: 2020 €</t>
-  </si>
-  <si>
-    <t>2020 €/$</t>
-  </si>
-  <si>
-    <t>BECCS</t>
-  </si>
-  <si>
-    <t>Source lost load</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1016/j.tej.2022.107187</t>
-  </si>
-  <si>
-    <t>Gorman. The quest to quantify the value of lost load: A critical review of the economics of power outages</t>
-  </si>
-  <si>
-    <t>https://atb-archive.nrel.gov/electricity/2020/data.php</t>
-  </si>
-  <si>
-    <t>NREL (National Renewable Energy Laboratory). 2020. "2020 Annual Technology Baseline."</t>
-  </si>
-  <si>
-    <t>Source BECCS</t>
-  </si>
-  <si>
-    <t>https://www.nrel.gov/docs/fy22osti/81644.pdf</t>
-  </si>
-  <si>
-    <t>CO2 emissions</t>
-  </si>
-  <si>
-    <t>tCO2/MWh</t>
-  </si>
-  <si>
-    <t>BECCS % link</t>
-  </si>
-  <si>
-    <t>beccs</t>
-  </si>
-  <si>
-    <t>beccs_out</t>
-  </si>
-  <si>
-    <t>Gorman</t>
-  </si>
-  <si>
-    <t>natgas_wCCS_out</t>
-  </si>
-  <si>
-    <t>Variable cost [€/MWh]</t>
-  </si>
-  <si>
-    <t>all_firm_case_currency_converted</t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1301,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1449,6 +1458,9 @@
     <xf numFmtId="49" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="19" fillId="45" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1526,6 +1538,9 @@
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Storage Techs"/>
       <sheetName val="Gravitational"/>
@@ -1533,7 +1548,13 @@
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0">
+        <row r="24">
+          <cell r="B24">
+            <v>3.1299847437582448E-3</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="12">
@@ -1847,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2173,18 +2194,18 @@
         <v>39</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>83</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>100</v>
-      </c>
       <c r="F26" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -2200,7 +2221,7 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -2208,7 +2229,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>143</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -2216,7 +2237,7 @@
         <v>36</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D30" t="s">
         <v>40</v>
@@ -2227,7 +2248,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2264,10 +2285,10 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B36" s="73" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.2">
@@ -2275,7 +2296,7 @@
         <v>42</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>101</v>
+        <v>196</v>
       </c>
       <c r="D37" t="s">
         <v>46</v>
@@ -2307,19 +2328,19 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="C42" s="1"/>
     </row>
@@ -2328,11 +2349,11 @@
         <v>64</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.2">
@@ -2348,16 +2369,16 @@
         <v>18</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K46" t="s">
         <v>69</v>
       </c>
       <c r="P46" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.2">
@@ -2365,7 +2386,7 @@
         <v>62</v>
       </c>
       <c r="J47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R47" t="s">
         <v>61</v>
@@ -2452,7 +2473,7 @@
         <v>76</v>
       </c>
       <c r="P50" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:26" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -2463,7 +2484,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>22</v>
@@ -2472,13 +2493,13 @@
         <v>33</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>43</v>
@@ -2496,7 +2517,7 @@
         <v>25</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="R51" s="2" t="s">
         <v>26</v>
@@ -2511,7 +2532,7 @@
         <v>60</v>
       </c>
       <c r="V51" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="X51" s="2" t="s">
         <v>27</v>
@@ -2526,7 +2547,7 @@
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E52" s="21"/>
       <c r="F52" s="21"/>
@@ -2563,11 +2584,11 @@
         <v>44</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -2589,7 +2610,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
@@ -2606,11 +2627,11 @@
         <v>44</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C54" s="22"/>
       <c r="D54" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
@@ -2632,7 +2653,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P54" s="22" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q54" s="22"/>
       <c r="R54" s="22"/>
@@ -2649,13 +2670,13 @@
         <v>44</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
@@ -2666,7 +2687,7 @@
       <c r="K55" s="18"/>
       <c r="L55" s="85">
         <f>M114*B33</f>
-        <v>143326.43376881725</v>
+        <v>163392.13449645168</v>
       </c>
       <c r="M55" s="18" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
@@ -2674,14 +2695,14 @@
       </c>
       <c r="N55" s="18">
         <f>P114</f>
-        <v>39.223057644110277</v>
+        <v>43.894285714285708</v>
       </c>
       <c r="O55" s="18" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P55" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="Q55" s="18"/>
       <c r="R55" s="18"/>
@@ -2698,19 +2719,19 @@
         <v>70</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G56" s="18"/>
       <c r="H56" s="18"/>
@@ -2732,7 +2753,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P56" s="18" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q56" s="18"/>
       <c r="R56" s="18"/>
@@ -2742,7 +2763,7 @@
       </c>
       <c r="U56" s="18"/>
       <c r="V56" s="17" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="W56" s="18" t="str">
         <f>B42 &amp; "/" &amp;B41 &amp; B40</f>
@@ -2756,13 +2777,13 @@
         <v>44</v>
       </c>
       <c r="B57" s="76" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C57" s="76" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D57" s="76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E57" s="76"/>
       <c r="F57" s="76"/>
@@ -2782,7 +2803,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P57" s="76" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q57" s="76"/>
       <c r="R57" s="76"/>
@@ -2799,19 +2820,19 @@
         <v>70</v>
       </c>
       <c r="B58" s="76" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C58" s="76" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D58" s="76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E58" s="76" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F58" s="76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G58" s="76"/>
       <c r="H58" s="76"/>
@@ -2833,7 +2854,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P58" s="76" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q58" s="76"/>
       <c r="R58" s="76"/>
@@ -2843,7 +2864,7 @@
       </c>
       <c r="U58" s="76"/>
       <c r="V58" s="75" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="W58" s="76" t="str">
         <f>B42 &amp; "/" &amp;B41 &amp; B40</f>
@@ -2857,13 +2878,13 @@
         <v>44</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
@@ -2874,7 +2895,7 @@
       <c r="K59" s="13"/>
       <c r="L59" s="89">
         <f>M118*B33</f>
-        <v>407013.04782420816</v>
+        <v>463994.87451959722</v>
       </c>
       <c r="M59" s="13" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
@@ -2882,14 +2903,14 @@
       </c>
       <c r="N59" s="13">
         <f>P118</f>
-        <v>14.561403508771932</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="O59" s="13" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P59" s="13" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="Q59" s="13"/>
       <c r="R59" s="13"/>
@@ -2906,19 +2927,19 @@
         <v>70</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
@@ -2940,7 +2961,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P60" s="13" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="Q60" s="13"/>
       <c r="R60" s="13"/>
@@ -2960,7 +2981,7 @@
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" s="23" t="s">
-        <v>44</v>
+        <v>193</v>
       </c>
       <c r="B61" s="24" t="s">
         <v>79</v>
@@ -2969,7 +2990,7 @@
         <v>79</v>
       </c>
       <c r="D61" s="24" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E61" s="24"/>
       <c r="F61" s="24"/>
@@ -2989,7 +3010,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P61" s="24" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q61" s="24"/>
       <c r="R61" s="24"/>
@@ -3003,22 +3024,22 @@
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" s="23" t="s">
-        <v>70</v>
+        <v>194</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C62" s="24" t="s">
         <v>79</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E62" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G62" s="24"/>
       <c r="H62" s="24"/>
@@ -3040,7 +3061,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P62" s="24" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q62" s="24"/>
       <c r="R62" s="24"/>
@@ -3050,7 +3071,7 @@
       </c>
       <c r="U62" s="24"/>
       <c r="V62" s="23" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="W62" s="24" t="str">
         <f>B42 &amp; "/" &amp;B41 &amp; B40</f>
@@ -3068,7 +3089,7 @@
       </c>
       <c r="C63" s="35"/>
       <c r="D63" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E63" s="35"/>
       <c r="F63" s="35"/>
@@ -3088,7 +3109,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P63" s="35" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q63" s="35"/>
       <c r="R63" s="35"/>
@@ -3102,14 +3123,14 @@
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
-        <v>44</v>
+        <v>193</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E64" s="15"/>
       <c r="F64" s="15"/>
@@ -3129,7 +3150,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P64" s="15" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q64" s="15"/>
       <c r="R64" s="15"/>
@@ -3143,14 +3164,14 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="25" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C65" s="26"/>
       <c r="D65" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E65" s="26"/>
       <c r="F65" s="26"/>
@@ -3175,7 +3196,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P65" s="26" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q65" s="26"/>
       <c r="R65" s="26">
@@ -3199,10 +3220,10 @@
         <v>32</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D66" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E66" s="28" t="s">
         <v>34</v>
@@ -3226,7 +3247,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P66" s="28" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q66" s="28"/>
       <c r="R66" s="28"/>
@@ -3243,10 +3264,10 @@
         <v>71</v>
       </c>
       <c r="B67" s="28" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D67" s="28" t="s">
         <v>34</v>
@@ -3269,11 +3290,13 @@
         <v>€/MWh</v>
       </c>
       <c r="P67" s="28" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q67" s="28"/>
       <c r="R67" s="28"/>
-      <c r="S67" s="28"/>
+      <c r="S67" s="28" t="b">
+        <v>1</v>
+      </c>
       <c r="T67" s="28"/>
       <c r="U67" s="28"/>
       <c r="V67" s="27"/>
@@ -3288,16 +3311,16 @@
         <v>70</v>
       </c>
       <c r="B68" s="28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D68" s="28" t="s">
         <v>34</v>
       </c>
       <c r="E68" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F68" s="28"/>
       <c r="G68" s="28"/>
@@ -3316,7 +3339,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P68" s="28" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q68" s="28"/>
       <c r="R68" s="28"/>
@@ -3333,16 +3356,16 @@
         <v>70</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C69" s="30" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F69" s="30"/>
       <c r="G69" s="30">
@@ -3354,7 +3377,7 @@
       <c r="K69" s="30"/>
       <c r="L69" s="31">
         <f>M112*B34</f>
-        <v>128512.40899070518</v>
+        <v>144749.35172885595</v>
       </c>
       <c r="M69" s="30" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
@@ -3362,14 +3385,14 @@
       </c>
       <c r="N69" s="30">
         <f>P112</f>
-        <v>2.631578947368421E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="O69" s="30" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P69" s="30" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="Q69" s="30"/>
       <c r="R69" s="30"/>
@@ -3381,7 +3404,7 @@
       <c r="X69" s="30"/>
       <c r="Y69" s="30"/>
       <c r="Z69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.2">
@@ -3389,13 +3412,13 @@
         <v>71</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C70" s="30" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D70" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E70" s="30"/>
       <c r="F70" s="30"/>
@@ -3406,7 +3429,7 @@
       <c r="K70" s="30"/>
       <c r="L70" s="31">
         <f>M111*B34</f>
-        <v>7417.7100155235103</v>
+        <v>8456.1894176967999</v>
       </c>
       <c r="M70" s="30" t="str">
         <f>B43 &amp; "/time range/" &amp; B41 &amp; B40</f>
@@ -3418,7 +3441,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P70" s="30" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="Q70" s="30"/>
       <c r="R70" s="30"/>
@@ -3430,7 +3453,7 @@
       <c r="X70" s="30"/>
       <c r="Y70" s="30"/>
       <c r="Z70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.2">
@@ -3438,11 +3461,11 @@
         <v>71</v>
       </c>
       <c r="B71" s="62" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C71" s="62"/>
       <c r="D71" s="62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E71" s="62"/>
       <c r="F71" s="62"/>
@@ -3453,7 +3476,7 @@
       <c r="K71" s="62"/>
       <c r="L71" s="80">
         <f>H121/8784*B34</f>
-        <v>219298.24561403508</v>
+        <v>250000</v>
       </c>
       <c r="M71" s="62" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
@@ -3465,7 +3488,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P71" s="62" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="Q71" s="62">
         <v>-1</v>
@@ -3484,11 +3507,11 @@
         <v>71</v>
       </c>
       <c r="B72" s="64" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C72" s="64"/>
       <c r="D72" s="64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E72" s="64"/>
       <c r="F72" s="64"/>
@@ -3499,7 +3522,7 @@
       <c r="K72" s="64"/>
       <c r="L72" s="81">
         <f>H121/8784*B34</f>
-        <v>219298.24561403508</v>
+        <v>250000</v>
       </c>
       <c r="M72" s="64" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
@@ -3511,7 +3534,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P72" s="64" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="Q72" s="64"/>
       <c r="R72" s="64"/>
@@ -3528,11 +3551,11 @@
         <v>44</v>
       </c>
       <c r="B73" s="72" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C73" s="72"/>
       <c r="D73" s="72" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E73" s="72"/>
       <c r="F73" s="72"/>
@@ -3548,14 +3571,14 @@
       </c>
       <c r="N73" s="72">
         <f>P120</f>
-        <v>8771.9298245614045</v>
+        <v>10000</v>
       </c>
       <c r="O73" s="72" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P73" s="72" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="Q73" s="72"/>
       <c r="R73" s="72"/>
@@ -3572,17 +3595,17 @@
         <v>70</v>
       </c>
       <c r="B74" s="70" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C74" s="70"/>
       <c r="D74" s="70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E74" s="70" t="s">
         <v>78</v>
       </c>
       <c r="F74" s="70" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G74" s="70"/>
       <c r="H74" s="70"/>
@@ -3600,7 +3623,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P74" s="70" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q74" s="70"/>
       <c r="R74" s="70"/>
@@ -3608,7 +3631,7 @@
       <c r="T74" s="70"/>
       <c r="U74" s="70"/>
       <c r="V74" s="69" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="W74" s="70" t="str">
         <f xml:space="preserve"> B41 &amp; B40  &amp; "/" &amp;  B42</f>
@@ -3622,11 +3645,11 @@
         <v>71</v>
       </c>
       <c r="B75" s="33" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C75" s="33"/>
       <c r="D75" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E75" s="33"/>
       <c r="F75" s="33"/>
@@ -3648,7 +3671,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P75" s="33" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="Q75" s="33"/>
       <c r="R75" s="33"/>
@@ -3665,7 +3688,7 @@
         <v>71</v>
       </c>
       <c r="B76" s="67" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C76" s="67"/>
       <c r="D76" s="67" t="s">
@@ -3686,7 +3709,7 @@
       <c r="N76" s="67"/>
       <c r="O76" s="67"/>
       <c r="P76" s="67" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q76" s="67"/>
       <c r="R76" s="67"/>
@@ -3723,22 +3746,22 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="88" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="37" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E88" s="36"/>
       <c r="F88" s="36"/>
@@ -3754,10 +3777,10 @@
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" s="37"/>
       <c r="B89" s="38" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C89" s="40" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E89" s="36"/>
       <c r="F89" s="36"/>
@@ -3774,7 +3797,7 @@
       <c r="A90" s="37"/>
       <c r="B90" s="39"/>
       <c r="C90" s="41" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E90" s="36"/>
       <c r="F90" s="36"/>
@@ -3805,10 +3828,10 @@
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" s="37"/>
       <c r="B92" s="38" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C92" s="68" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E92" s="36"/>
       <c r="F92" s="36"/>
@@ -3825,7 +3848,7 @@
       <c r="A93" s="37"/>
       <c r="B93" s="38"/>
       <c r="C93" s="79" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E93" s="36"/>
       <c r="F93" s="36"/>
@@ -3856,10 +3879,10 @@
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" s="37"/>
       <c r="B95" s="38" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C95" s="86" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E95" s="36"/>
       <c r="F95" s="36"/>
@@ -3876,7 +3899,7 @@
       <c r="A96" s="37"/>
       <c r="B96" s="38"/>
       <c r="C96" s="79" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E96" s="36"/>
       <c r="F96" s="36"/>
@@ -3912,10 +3935,10 @@
     <row r="98" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="37"/>
       <c r="B98" s="38" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C98" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E98" s="36"/>
       <c r="F98" s="36"/>
@@ -3932,7 +3955,7 @@
       <c r="A99" s="37"/>
       <c r="B99" s="38"/>
       <c r="C99" s="65" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E99" s="36"/>
       <c r="F99" s="36"/>
@@ -3963,10 +3986,10 @@
     <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" s="37"/>
       <c r="B101" s="38" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C101" s="86" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E101" s="36"/>
       <c r="F101" s="36"/>
@@ -3983,7 +4006,7 @@
       <c r="A102" s="37"/>
       <c r="B102" s="38"/>
       <c r="C102" s="65" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E102" s="36"/>
       <c r="F102" s="36"/>
@@ -4012,10 +4035,10 @@
     <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" s="37"/>
       <c r="B104" s="38" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C104" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F104" s="36"/>
       <c r="G104" s="36"/>
@@ -4031,7 +4054,7 @@
       <c r="A105" s="37"/>
       <c r="B105" s="38"/>
       <c r="C105" s="39" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F105" s="36"/>
       <c r="G105" s="36"/>
@@ -4074,12 +4097,14 @@
     <row r="108" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="37"/>
       <c r="B108" s="42" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C108" s="43">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="D108" s="44"/>
+        <v>1</v>
+      </c>
+      <c r="D108" s="90" t="s">
+        <v>192</v>
+      </c>
       <c r="E108" s="44"/>
       <c r="F108" s="44"/>
       <c r="G108" s="45"/>
@@ -4098,7 +4123,7 @@
     <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" s="37"/>
       <c r="B109" s="46" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C109" s="45">
         <v>7.0000000000000007E-2</v>
@@ -4133,13 +4158,13 @@
         <v>Fixed O&amp;M cost [€/MWyear]</v>
       </c>
       <c r="E110" s="47" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F110" s="47" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G110" s="47" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H110" s="49" t="str">
         <f xml:space="preserve"> "Annual fixed costs [" &amp;B43 &amp; "/year]"</f>
@@ -4154,27 +4179,27 @@
         <v>Fuel cost [€/MWh]</v>
       </c>
       <c r="K110" s="46" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="L110" s="46" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="M110" s="48" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="N110" s="47"/>
       <c r="O110" s="47"/>
       <c r="P110" s="48" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="Q110" s="88" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="R110" s="87"/>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B111" s="45" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C111" s="50">
         <f>103100</f>
@@ -4202,7 +4227,7 @@
       <c r="L111" s="45"/>
       <c r="M111" s="50">
         <f>H111/8760/C108</f>
-        <v>0.84445696898036315</v>
+        <v>0.96268094463761389</v>
       </c>
       <c r="N111" s="45" t="str">
         <f>B43 &amp; "/" &amp; B40 &amp; "/" &amp; B41</f>
@@ -4215,7 +4240,7 @@
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B112" s="51" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C112" s="45">
         <f>1612000</f>
@@ -4223,7 +4248,7 @@
       </c>
       <c r="D112" s="45">
         <f>12500*C108</f>
-        <v>14249.999999999998</v>
+        <v>12500</v>
       </c>
       <c r="E112" s="52">
         <v>1.4999999999999999E-2</v>
@@ -4237,7 +4262,7 @@
       </c>
       <c r="H112" s="51">
         <f>((C112+E112*C112)*G112+D112)</f>
-        <v>146103.86169680991</v>
+        <v>144353.86169680991</v>
       </c>
       <c r="I112" s="50"/>
       <c r="J112" s="45"/>
@@ -4247,7 +4272,7 @@
       <c r="L112" s="45"/>
       <c r="M112" s="50">
         <f>H112/8760/C108</f>
-        <v>14.630283355043851</v>
+        <v>16.478751335252273</v>
       </c>
       <c r="N112" s="45" t="str">
         <f>B43 &amp; "/" &amp; B40 &amp; "/" &amp; B41</f>
@@ -4256,7 +4281,7 @@
       <c r="O112" s="45"/>
       <c r="P112" s="50">
         <f>0.0003/C108</f>
-        <v>2.631578947368421E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="Q112" s="87"/>
       <c r="R112" s="87"/>
@@ -4282,7 +4307,7 @@
     </row>
     <row r="114" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B114" s="51" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C114" s="45">
         <v>1969000</v>
@@ -4303,7 +4328,8 @@
         <v>162945.70789946683</v>
       </c>
       <c r="I114" s="45">
-        <v>9</v>
+        <f>2*4.09</f>
+        <v>8.18</v>
       </c>
       <c r="J114" s="45">
         <v>20</v>
@@ -4314,7 +4340,7 @@
       <c r="L114" s="45"/>
       <c r="M114" s="50">
         <f>H114/8760/C108</f>
-        <v>16.31676158570324</v>
+        <v>18.601108207701692</v>
       </c>
       <c r="N114" s="45" t="str">
         <f>B43 &amp; "/" &amp; B40 &amp; "/" &amp; B41</f>
@@ -4323,14 +4349,14 @@
       <c r="O114" s="51"/>
       <c r="P114" s="45">
         <f>(I114+J114/K114)/C108</f>
-        <v>39.223057644110277</v>
+        <v>43.894285714285708</v>
       </c>
       <c r="Q114" s="87"/>
       <c r="R114" s="87"/>
     </row>
     <row r="115" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B115" s="45" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C115" s="45"/>
       <c r="D115" s="45"/>
@@ -4381,13 +4407,13 @@
       <c r="L116" s="45"/>
       <c r="M116" s="50">
         <f>H116/8760/C108</f>
-        <v>8.0050581073281979</v>
+        <v>9.1257662423541444</v>
       </c>
       <c r="N116" s="45"/>
       <c r="O116" s="45"/>
       <c r="P116" s="45">
         <f>(I116+J116/K116)/C108</f>
-        <v>14.285714285714286</v>
+        <v>16.285714285714285</v>
       </c>
       <c r="Q116" s="87"/>
       <c r="R116" s="87"/>
@@ -4413,7 +4439,7 @@
     </row>
     <row r="118" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B118" s="45" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C118" s="45">
         <v>5580000</v>
@@ -4439,7 +4465,7 @@
       <c r="L118" s="45"/>
       <c r="M118" s="50">
         <f>H118/8760/C108</f>
-        <v>46.335729488183986</v>
+        <v>52.822731616529737</v>
       </c>
       <c r="N118" s="45" t="str">
         <f>B43 &amp; "/" &amp; B40 &amp; "/" &amp; B41</f>
@@ -4448,13 +4474,13 @@
       <c r="O118" s="45"/>
       <c r="P118" s="45">
         <f>16.6/C108</f>
-        <v>14.561403508771932</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="Q118" s="87">
         <v>-1.22</v>
       </c>
       <c r="R118" s="87" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="119" spans="2:18" x14ac:dyDescent="0.2">
@@ -4478,7 +4504,7 @@
     </row>
     <row r="120" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B120" s="45" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C120" s="45"/>
       <c r="D120" s="45"/>
@@ -4495,14 +4521,14 @@
       <c r="O120" s="45"/>
       <c r="P120" s="45">
         <f>10000/C108</f>
-        <v>8771.9298245614045</v>
+        <v>10000</v>
       </c>
       <c r="Q120" s="87"/>
       <c r="R120" s="87"/>
     </row>
     <row r="121" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B121" s="45" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C121" s="45"/>
       <c r="D121" s="45"/>
@@ -4511,7 +4537,7 @@
       <c r="G121" s="45"/>
       <c r="H121" s="45">
         <f>250000/C108</f>
-        <v>219298.24561403511</v>
+        <v>250000</v>
       </c>
       <c r="I121" s="45"/>
       <c r="J121" s="45"/>
@@ -4526,7 +4552,7 @@
     </row>
     <row r="123" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="125" spans="2:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
cleaned up component removal
</commit_message>
<xml_diff>
--- a/all_firm_case.xlsx
+++ b/all_firm_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/Library/Group Containers/G69SCX94XU.duck/Library/Application Support/duck/Volumes.noindex/DPB-DGE Data Transfer Node/nobackup/scratch/awongel/clab_all_firm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D8CD35-41DD-3E43-BFEC-056472B91414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576B084B-7F4D-CA4F-842A-5F81702B9AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -840,10 +840,10 @@
     <t>all_firm_case</t>
   </si>
   <si>
-    <t>/input_data/costs_2020.csv</t>
-  </si>
-  <si>
-    <t>/input_data/</t>
+    <t>input_data/</t>
+  </si>
+  <si>
+    <t>input_data/costs_2020.csv</t>
   </si>
 </sst>
 </file>
@@ -2196,7 +2196,7 @@
   <dimension ref="A1:Z167"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2521,7 +2521,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -2529,7 +2529,7 @@
         <v>98</v>
       </c>
       <c r="B26" s="86" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G26" t="s">
         <v>153</v>

</xml_diff>